<commit_message>
Before making first revision.
</commit_message>
<xml_diff>
--- a/doc/pots.xlsx
+++ b/doc/pots.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E.Walbach\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.hallab\projects\ScienceDbBackend\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="14820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6816"/>
   </bookViews>
   <sheets>
     <sheet name="pots" sheetId="1" r:id="rId1"/>
@@ -1103,19 +1103,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.68359375" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.15625" customWidth="1"/>
+    <col min="4" max="4" width="17.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1269,7 +1269,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>28</v>
       </c>

</xml_diff>